<commit_message>
TimeStorage zaman olayini cozmek icin eklendi. Derslerin veritabanina atilimi tamamlandi
</commit_message>
<xml_diff>
--- a/taas/TAAS EXCEL.xlsx
+++ b/taas/TAAS EXCEL.xlsx
@@ -143,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -155,14 +155,14 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
       <sz val="10"/>
@@ -173,6 +173,11 @@
       <sz val="0"/>
       <color indexed="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
     </font>
     <font>
       <u val="single"/>
@@ -218,12 +223,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -231,20 +236,17 @@
     <xf numFmtId="1" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1531,7 +1533,7 @@
         <v>131</v>
       </c>
       <c r="C2" s="5">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1656,10 +1658,10 @@
       <c r="F1" t="s" s="5">
         <v>10</v>
       </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="5">
@@ -1680,10 +1682,10 @@
       <c r="F2" t="s" s="5">
         <v>15</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
@@ -1704,10 +1706,10 @@
       <c r="F3" t="s" s="5">
         <v>20</v>
       </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" ht="15.65" customHeight="1">
       <c r="A4" s="4"/>
@@ -1817,14 +1819,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="8" customWidth="1"/>
-    <col min="3" max="3" width="18.375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="8" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="8" customWidth="1"/>
-    <col min="7" max="7" width="25.75" style="8" customWidth="1"/>
-    <col min="8" max="256" width="10.875" style="8" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="18.375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="25.75" style="7" customWidth="1"/>
+    <col min="8" max="256" width="10.875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">

</xml_diff>

<commit_message>
teaches tablosu artık doluyor
</commit_message>
<xml_diff>
--- a/taas/TAAS EXCEL.xlsx
+++ b/taas/TAAS EXCEL.xlsx
@@ -65,7 +65,7 @@
     </r>
   </si>
   <si>
-    <t>COMP 131, COMP 302</t>
+    <t>COMP 131,COMP 302</t>
   </si>
   <si>
     <t>Java</t>
@@ -88,7 +88,7 @@
     </r>
   </si>
   <si>
-    <t>ELEC 201</t>
+    <t>ELEC 201,ELEC 204</t>
   </si>
   <si>
     <t>Matlab</t>
@@ -1565,9 +1565,15 @@
       <c r="E4" s="4"/>
     </row>
     <row r="5" ht="15.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
+      <c r="A5" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4">
+        <v>204</v>
+      </c>
+      <c r="C5" s="4">
+        <v>45</v>
+      </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
     </row>

</xml_diff>

<commit_message>
Asistan ve advisor iliksis yapildi. Asistanlar db'ye ekleniyor.
</commit_message>
<xml_diff>
--- a/taas/TAAS EXCEL.xlsx
+++ b/taas/TAAS EXCEL.xlsx
@@ -112,13 +112,21 @@
     <t>ocetinkaya13@ku.edu.tr</t>
   </si>
   <si>
-    <t>akan@ku.edu.tr</t>
-  </si>
-  <si>
-    <t>Signal, Matlab</t>
-  </si>
-  <si>
-    <t>PHYS 101</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>doztreves@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>Signal,Matlab</t>
+  </si>
+  <si>
+    <t>ELEC 201,COMP 131</t>
   </si>
   <si>
     <t>Farideh</t>
@@ -130,10 +138,18 @@
     <t>fhalaku@ku.edu.tr</t>
   </si>
   <si>
-    <t>stasiran@ku.edu.tr</t>
-  </si>
-  <si>
-    <t>COMP 131</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>mpinar@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>COMP 302,ELEC 204</t>
   </si>
 </sst>
 </file>
@@ -143,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -183,6 +199,12 @@
       <u val="single"/>
       <sz val="0"/>
       <color indexed="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="0"/>
+      <color indexed="11"/>
       <name val="Verdana"/>
     </font>
   </fonts>
@@ -267,6 +289,7 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff009999"/>
+      <rgbColor rgb="ff0000ff"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -1968,6 +1991,10 @@
       <c r="G10" s="4"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="E3" r:id="rId2" location="" tooltip="" display=""/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
Existing instructor olayi handle edildi
</commit_message>
<xml_diff>
--- a/taas/TAAS EXCEL.xlsx
+++ b/taas/TAAS EXCEL.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>KODU</t>
   </si>
@@ -42,7 +42,7 @@
     <t>DEPARTMENT</t>
   </si>
   <si>
-    <t>COURSES</t>
+    <t>TEACHING</t>
   </si>
   <si>
     <t>ADDITIONAL REQUEST</t>
@@ -65,10 +65,16 @@
     </r>
   </si>
   <si>
-    <t>COMP 131,COMP 302</t>
+    <t>COMP 302</t>
   </si>
   <si>
     <t>Java</t>
+  </si>
+  <si>
+    <t>COMP 131</t>
+  </si>
+  <si>
+    <t>GRASP</t>
   </si>
   <si>
     <t>Ozgur Baris</t>
@@ -88,10 +94,13 @@
     </r>
   </si>
   <si>
-    <t>ELEC 201,ELEC 204</t>
+    <t>ELEC 201</t>
   </si>
   <si>
     <t>Matlab</t>
+  </si>
+  <si>
+    <t>ELEC 204</t>
   </si>
   <si>
     <t>ADVISOR MAIL</t>
@@ -1649,7 +1658,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1718,51 +1727,75 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s" s="5">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s" s="5">
         <v>16</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="F3" t="s" s="5">
         <v>17</v>
-      </c>
-      <c r="C3" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="F3" t="s" s="5">
-        <v>20</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" ht="15.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+    <row r="4" ht="20" customHeight="1">
+      <c r="A4" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="E4" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
     </row>
     <row r="5" ht="15.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="A5" t="s" s="5">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="5">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" ht="15.65" customHeight="1">
       <c r="A6" s="4"/>
@@ -1824,10 +1857,24 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
+    <row r="11" ht="15.65" customHeight="1">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="C5" r:id="rId4" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1872,59 +1919,59 @@
         <v>8</v>
       </c>
       <c r="E1" t="s" s="5">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F1" t="s" s="5">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="G1" t="s" s="5">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s" s="5">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s" s="5">
         <v>3</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s" s="5">
         <v>15</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" ht="15.65" customHeight="1">

</xml_diff>

<commit_message>
Background parse islemleri yapildi.
</commit_message>
<xml_diff>
--- a/taas/TAAS EXCEL.xlsx
+++ b/taas/TAAS EXCEL.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
   <si>
     <t>KODU</t>
   </si>
@@ -43,9 +43,6 @@
   </si>
   <si>
     <t>TEACHING</t>
-  </si>
-  <si>
-    <t>ADDITIONAL REQUEST</t>
   </si>
   <si>
     <t>Serdar</t>
@@ -65,16 +62,7 @@
     </r>
   </si>
   <si>
-    <t>COMP 302</t>
-  </si>
-  <si>
-    <t>Java</t>
-  </si>
-  <si>
-    <t>COMP 131</t>
-  </si>
-  <si>
-    <t>GRASP</t>
+    <t>COMP 302, COMP 131</t>
   </si>
   <si>
     <t>Ozgur Baris</t>
@@ -94,13 +82,7 @@
     </r>
   </si>
   <si>
-    <t>ELEC 201</t>
-  </si>
-  <si>
-    <t>Matlab</t>
-  </si>
-  <si>
-    <t>ELEC 204</t>
+    <t>ELEC 201,ELEC 204</t>
   </si>
   <si>
     <t>ADVISOR MAIL</t>
@@ -156,6 +138,9 @@
       </rPr>
       <t>mpinar@ku.edu.tr</t>
     </r>
+  </si>
+  <si>
+    <t>Java, GRASP</t>
   </si>
   <si>
     <t>COMP 302,ELEC 204</t>
@@ -254,7 +239,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -275,6 +260,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
@@ -1658,7 +1646,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1693,9 +1681,7 @@
       <c r="E1" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="F1" t="s" s="5">
-        <v>10</v>
-      </c>
+      <c r="F1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1703,23 +1689,21 @@
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s" s="5">
         <v>11</v>
       </c>
-      <c r="B2" t="s" s="5">
+      <c r="C2" t="s" s="5">
         <v>12</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>13</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>3</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s" s="5">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1727,75 +1711,49 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>16</v>
-      </c>
-      <c r="F3" t="s" s="5">
         <v>17</v>
       </c>
+      <c r="F3" s="7"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" ht="20" customHeight="1">
-      <c r="A4" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="E4" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s" s="5">
-        <v>22</v>
-      </c>
+    <row r="4" ht="15.65" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" ht="15.65" customHeight="1">
-      <c r="A5" t="s" s="5">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s" s="5">
-        <v>19</v>
-      </c>
-      <c r="C5" t="s" s="5">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s" s="5">
-        <v>4</v>
-      </c>
-      <c r="E5" t="s" s="5">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s" s="5">
-        <v>22</v>
-      </c>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
     </row>
     <row r="6" ht="15.65" customHeight="1">
       <c r="A6" s="4"/>
@@ -1857,24 +1815,10 @@
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" ht="15.65" customHeight="1">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display=""/>
-    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display=""/>
-    <hyperlink ref="C5" r:id="rId4" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1895,14 +1839,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="7" customWidth="1"/>
-    <col min="3" max="3" width="18.375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="7" customWidth="1"/>
-    <col min="6" max="6" width="12.875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="25.75" style="7" customWidth="1"/>
-    <col min="8" max="256" width="10.875" style="7" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="8" customWidth="1"/>
+    <col min="3" max="3" width="18.375" style="8" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="11.75" style="8" customWidth="1"/>
+    <col min="6" max="6" width="12.875" style="8" customWidth="1"/>
+    <col min="7" max="7" width="25.75" style="8" customWidth="1"/>
+    <col min="8" max="256" width="10.875" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
@@ -1919,59 +1863,59 @@
         <v>8</v>
       </c>
       <c r="E1" t="s" s="5">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="F1" t="s" s="5">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="G1" t="s" s="5">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F2" t="s" s="5">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s" s="5">
         <v>3</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s" s="5">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s" s="5">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" ht="15.65" customHeight="1">

</xml_diff>

<commit_message>
ne degisiklikler var bilmiyorum
</commit_message>
<xml_diff>
--- a/taas/TAAS EXCEL.xlsx
+++ b/taas/TAAS EXCEL.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="66">
   <si>
     <t>KODU</t>
   </si>
@@ -28,6 +28,12 @@
   </si>
   <si>
     <t>ELEC</t>
+  </si>
+  <si>
+    <t>INDR</t>
+  </si>
+  <si>
+    <t>CHBI</t>
   </si>
   <si>
     <t>NAME</t>
@@ -85,6 +91,46 @@
     <t>ELEC 201,ELEC 204</t>
   </si>
   <si>
+    <t>Ceyda</t>
+  </si>
+  <si>
+    <t>Oguz</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>dsadsa@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>INDR 440</t>
+  </si>
+  <si>
+    <t>Ibrahim</t>
+  </si>
+  <si>
+    <t>Baris</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>qwerty@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>CHBI 200</t>
+  </si>
+  <si>
     <t>ADVISOR MAIL</t>
   </si>
   <si>
@@ -94,13 +140,21 @@
     <t>PREVIOUS TEACHING (LAST 4 SEM)</t>
   </si>
   <si>
-    <t>Oktay</t>
-  </si>
-  <si>
-    <t>Cetinkaya</t>
-  </si>
-  <si>
-    <t>ocetinkaya13@ku.edu.tr</t>
+    <t>Asistan</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a1@ku.edu.tr</t>
+    </r>
   </si>
   <si>
     <r>
@@ -120,13 +174,7 @@
     <t>ELEC 201,COMP 131</t>
   </si>
   <si>
-    <t>Farideh</t>
-  </si>
-  <si>
-    <t>Halakou</t>
-  </si>
-  <si>
-    <t>fhalaku@ku.edu.tr</t>
+    <t>b</t>
   </si>
   <si>
     <r>
@@ -136,6 +184,48 @@
         <color indexed="11"/>
         <rFont val="Verdana"/>
       </rPr>
+      <t>a2@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>doztreves@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>Xilinx</t>
+  </si>
+  <si>
+    <t>COMP 302,ELEC 204</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a3@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="11"/>
+        <rFont val="Arial"/>
+      </rPr>
       <t>mpinar@ku.edu.tr</t>
     </r>
   </si>
@@ -143,7 +233,104 @@
     <t>Java, GRASP</t>
   </si>
   <si>
-    <t>COMP 302,ELEC 204</t>
+    <t>COMP 202</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a4@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>COMP 416</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a5@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a6@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>Optimization</t>
+  </si>
+  <si>
+    <t>INDR 100</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a7@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>Organic Chemistry</t>
+  </si>
+  <si>
+    <t>CHBI 100</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="0"/>
+        <color indexed="11"/>
+        <rFont val="Verdana"/>
+      </rPr>
+      <t>a8@ku.edu.tr</t>
+    </r>
+  </si>
+  <si>
+    <t>qwerty@ku.edu.tr</t>
+  </si>
+  <si>
+    <t>DNA</t>
   </si>
 </sst>
 </file>
@@ -153,7 +340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -201,6 +388,18 @@
       <color indexed="11"/>
       <name val="Verdana"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color indexed="11"/>
+      <name val="Verdana"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -239,7 +438,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -258,13 +457,16 @@
     <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
+    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1598,16 +1800,28 @@
       <c r="E5" s="4"/>
     </row>
     <row r="6" ht="15.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4">
+        <v>440</v>
+      </c>
+      <c r="C6" s="4">
+        <v>40</v>
+      </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
     <row r="7" ht="15.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4">
+        <v>200</v>
+      </c>
+      <c r="C7" s="4">
+        <v>100</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
@@ -1652,36 +1866,36 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="10.875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="6" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="6" customWidth="1"/>
-    <col min="5" max="5" width="17.5" style="6" customWidth="1"/>
-    <col min="6" max="6" width="21.875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="21.875" style="6" customWidth="1"/>
-    <col min="8" max="8" width="21.875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="21.875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="21.875" style="6" customWidth="1"/>
-    <col min="11" max="256" width="10.875" style="6" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="10.875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="7" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="21.875" style="7" customWidth="1"/>
+    <col min="8" max="8" width="21.875" style="7" customWidth="1"/>
+    <col min="9" max="9" width="21.875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="21.875" style="7" customWidth="1"/>
+    <col min="11" max="256" width="10.875" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" t="s" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s" s="5">
-        <v>9</v>
-      </c>
-      <c r="F1" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
@@ -1689,21 +1903,21 @@
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>3</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="F2" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1711,44 +1925,64 @@
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D3" t="s" s="5">
         <v>4</v>
       </c>
       <c r="E3" t="s" s="5">
-        <v>17</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>19</v>
+      </c>
+      <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
     <row r="4" ht="15.65" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
+      <c r="A4" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" t="s" s="5">
+        <v>23</v>
+      </c>
+      <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
     <row r="5" ht="15.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="A5" t="s" s="6">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s" s="6">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>27</v>
+      </c>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -1819,6 +2053,8 @@
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
     <hyperlink ref="C3" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="C4" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="C5" r:id="rId4" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -1843,7 +2079,7 @@
     <col min="2" max="2" width="10.875" style="8" customWidth="1"/>
     <col min="3" max="3" width="18.375" style="8" customWidth="1"/>
     <col min="4" max="4" width="10.875" style="8" customWidth="1"/>
-    <col min="5" max="5" width="11.75" style="8" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="8" customWidth="1"/>
     <col min="6" max="6" width="12.875" style="8" customWidth="1"/>
     <col min="7" max="7" width="25.75" style="8" customWidth="1"/>
     <col min="8" max="256" width="10.875" style="8" customWidth="1"/>
@@ -1851,125 +2087,207 @@
   <sheetData>
     <row r="1" ht="20" customHeight="1">
       <c r="A1" t="s" s="5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" t="s" s="5">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s" s="5">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D1" t="s" s="5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E1" t="s" s="5">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s" s="5">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s" s="5">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" ht="20" customHeight="1">
       <c r="A2" t="s" s="5">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s" s="5">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s" s="5">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D2" t="s" s="5">
         <v>4</v>
       </c>
       <c r="E2" t="s" s="5">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s" s="5">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s" s="5">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" ht="20" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s" s="5">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s" s="5">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s" s="5">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s" s="9">
+        <v>40</v>
+      </c>
+      <c r="G3" t="s" s="5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" ht="15.65" customHeight="1">
+      <c r="A4" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s" s="5">
+        <v>42</v>
+      </c>
+      <c r="C4" t="s" s="5">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s" s="6">
         <v>3</v>
       </c>
-      <c r="E3" t="s" s="5">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s" s="5">
+      <c r="E4" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s" s="5">
+        <v>45</v>
+      </c>
+      <c r="G4" t="s" s="6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" ht="15.65" customHeight="1">
+      <c r="A5" t="s" s="5">
         <v>31</v>
       </c>
-      <c r="G3" t="s" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" ht="15.65" customHeight="1">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" ht="15.65" customHeight="1">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" t="s" s="5">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s" s="6">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s" s="6">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s" s="6">
+        <v>49</v>
+      </c>
+      <c r="G5" t="s" s="6">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" ht="15.65" customHeight="1">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="A6" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s" s="5">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s" s="5">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="6">
+        <v>53</v>
+      </c>
+      <c r="G6" t="s" s="6">
+        <v>23</v>
+      </c>
     </row>
     <row r="7" ht="15.65" customHeight="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="A7" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s" s="5">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s" s="6">
+        <v>5</v>
+      </c>
+      <c r="E7" t="s" s="5">
+        <v>22</v>
+      </c>
+      <c r="F7" t="s" s="6">
+        <v>56</v>
+      </c>
+      <c r="G7" t="s" s="6">
+        <v>57</v>
+      </c>
     </row>
     <row r="8" ht="15.65" customHeight="1">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="A8" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s" s="5">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s" s="5">
+        <v>59</v>
+      </c>
+      <c r="D8" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s" s="6">
+        <v>26</v>
+      </c>
+      <c r="F8" t="s" s="6">
+        <v>60</v>
+      </c>
+      <c r="G8" t="s" s="6">
+        <v>61</v>
+      </c>
     </row>
     <row r="9" ht="15.65" customHeight="1">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
+      <c r="A9" t="s" s="5">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s" s="5">
+        <v>62</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s" s="6">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s" s="6">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s" s="6">
+        <v>65</v>
+      </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" ht="15.65" customHeight="1">
@@ -1983,8 +2301,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" location="" tooltip="" display=""/>
-    <hyperlink ref="E3" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="C2" r:id="rId1" location="" tooltip="" display=""/>
+    <hyperlink ref="E2" r:id="rId2" location="" tooltip="" display=""/>
+    <hyperlink ref="C3" r:id="rId3" location="" tooltip="" display=""/>
+    <hyperlink ref="E3" r:id="rId4" location="" tooltip="" display=""/>
+    <hyperlink ref="C4" r:id="rId5" location="" tooltip="" display=""/>
+    <hyperlink ref="E4" r:id="rId6" location="" tooltip="" display=""/>
+    <hyperlink ref="C5" r:id="rId7" location="" tooltip="" display=""/>
+    <hyperlink ref="E5" r:id="rId8" location="" tooltip="" display=""/>
+    <hyperlink ref="C6" r:id="rId9" location="" tooltip="" display=""/>
+    <hyperlink ref="E6" r:id="rId10" location="" tooltip="" display=""/>
+    <hyperlink ref="C7" r:id="rId11" location="" tooltip="" display=""/>
+    <hyperlink ref="E7" r:id="rId12" location="" tooltip="" display=""/>
+    <hyperlink ref="C8" r:id="rId13" location="" tooltip="" display=""/>
+    <hyperlink ref="E8" r:id="rId14" location="" tooltip="" display=""/>
+    <hyperlink ref="C9" r:id="rId15" location="" tooltip="" display=""/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>